<commit_message>
fixing prep proportion error
</commit_message>
<xml_diff>
--- a/applications/SHIELD/Documentation/Syphilis Manager Data Overview_2.19.26.xlsx
+++ b/applications/SHIELD/Documentation/Syphilis Manager Data Overview_2.19.26.xlsx
@@ -1475,9 +1475,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M71" sqref="M71"/>
+      <selection pane="bottomLeft" activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>